<commit_message>
Data Driven Framework 1
</commit_message>
<xml_diff>
--- a/wcsm9automationproject/src/main/resources/ActiTimeTestData.xlsx
+++ b/wcsm9automationproject/src/main/resources/ActiTimeTestData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19332" windowHeight="4944" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="validcreds" sheetId="1" r:id="rId1"/>
     <sheet name="invalidcreds" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>